<commit_message>
Envio de emails sem necessidade do excel scope
</commit_message>
<xml_diff>
--- a/config/E-mails para Notificações – RPA.xlsx
+++ b/config/E-mails para Notificações – RPA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Squad2\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA34D43-A0E3-4BE2-92CC-1CF179453B57}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014B9ADD-88C7-4A1B-B7CE-CAF73189DA98}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{CAADC2FD-21F2-4A27-AAD9-DD36690C542D}"/>
   </bookViews>
@@ -30,13 +30,13 @@
     <t>E-mails</t>
   </si>
   <si>
+    <t>lucas.araj.contato@gmail.com</t>
+  </si>
+  <si>
     <t>caioav99@gmail.com</t>
   </si>
   <si>
     <t>caioav63@gmail.com</t>
-  </si>
-  <si>
-    <t>lucas.araj.contato@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,11 +440,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{219FD375-27EA-4BA0-9D76-F6318671CFE3}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{60B278D2-668E-4A07-8901-ACD5A57E10FF}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{43558F4B-5B9E-47E8-84A7-76C964053734}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add email do caio na planilha
</commit_message>
<xml_diff>
--- a/config/E-mails para Notificações – RPA.xlsx
+++ b/config/E-mails para Notificações – RPA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Squad2\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014B9ADD-88C7-4A1B-B7CE-CAF73189DA98}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD98A7C-70DD-4E3C-89C8-F907B7EAF81E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{CAADC2FD-21F2-4A27-AAD9-DD36690C542D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>E-mails</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>caioav63@gmail.com</t>
+  </si>
+  <si>
+    <t>eng.caio.camilo@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -408,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAC9A782-2F7B-4B26-ACB6-C278FA6821F5}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,7 +442,15 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A5" r:id="rId1" xr:uid="{86A2F7DC-4DF6-42F6-8825-AB3358CF5208}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>